<commit_message>
Cleaned raw clearance Excel to csv
</commit_message>
<xml_diff>
--- a/data/raw_data.xlsx
+++ b/data/raw_data.xlsx
@@ -19715,8 +19715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G98" sqref="G98"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D135" sqref="D135:D136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>